<commit_message>
Add WP3 variable: distance to meteorological station (mdist) to the non-repeated, trimester repeated and yearly repeated dictionaries
</commit_message>
<xml_diff>
--- a/dictionaries/core/2_2/2_2_non_rep.xlsx
+++ b/dictionaries/core/2_2/2_2_non_rep.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16416" activeTab="1"/>
+    <workbookView xWindow="-12" yWindow="12" windowWidth="12144" windowHeight="12864"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="852">
   <si>
     <t>name</t>
   </si>
@@ -2565,6 +2565,12 @@
   </si>
   <si>
     <t>Child's born abroad</t>
+  </si>
+  <si>
+    <t>mdist_preg</t>
+  </si>
+  <si>
+    <t>distance to meteorological station during pregnancy</t>
   </si>
 </sst>
 </file>
@@ -2976,15 +2982,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D328"/>
+  <dimension ref="A1:D329"/>
   <sheetViews>
-    <sheetView topLeftCell="A298" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C328" sqref="C328"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="197.109375" style="1" bestFit="1" customWidth="1"/>
@@ -5817,21 +5823,21 @@
     </row>
     <row r="203" spans="1:4" ht="15" customHeight="1">
       <c r="A203" s="2" t="s">
-        <v>202</v>
+        <v>850</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>554</v>
+        <v>851</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="15" customHeight="1">
       <c r="A204" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>314</v>
@@ -5840,12 +5846,12 @@
         <v>343</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15" customHeight="1">
       <c r="A205" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>314</v>
@@ -5854,12 +5860,12 @@
         <v>343</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15" customHeight="1">
       <c r="A206" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>314</v>
@@ -5868,12 +5874,12 @@
         <v>343</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15" customHeight="1">
       <c r="A207" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>314</v>
@@ -5882,12 +5888,12 @@
         <v>343</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15" customHeight="1">
       <c r="A208" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>314</v>
@@ -5896,12 +5902,12 @@
         <v>343</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15" customHeight="1">
       <c r="A209" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>314</v>
@@ -5910,12 +5916,12 @@
         <v>343</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="15" customHeight="1">
       <c r="A210" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>314</v>
@@ -5924,12 +5930,12 @@
         <v>343</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15" customHeight="1">
       <c r="A211" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>314</v>
@@ -5938,12 +5944,12 @@
         <v>343</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="15" customHeight="1">
       <c r="A212" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>314</v>
@@ -5952,12 +5958,12 @@
         <v>343</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="15" customHeight="1">
       <c r="A213" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>314</v>
@@ -5966,12 +5972,12 @@
         <v>343</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="15" customHeight="1">
       <c r="A214" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>314</v>
@@ -5980,12 +5986,12 @@
         <v>343</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="15" customHeight="1">
       <c r="A215" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>314</v>
@@ -5994,12 +6000,12 @@
         <v>343</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="15" customHeight="1">
       <c r="A216" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>314</v>
@@ -6008,12 +6014,12 @@
         <v>343</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="15" customHeight="1">
       <c r="A217" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>314</v>
@@ -6022,12 +6028,12 @@
         <v>343</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="15" customHeight="1">
       <c r="A218" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>314</v>
@@ -6036,12 +6042,12 @@
         <v>343</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="15" customHeight="1">
       <c r="A219" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>314</v>
@@ -6050,12 +6056,12 @@
         <v>343</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="15" customHeight="1">
       <c r="A220" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>314</v>
@@ -6064,54 +6070,54 @@
         <v>343</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="15" customHeight="1">
       <c r="A221" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>316</v>
+        <v>343</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15" customHeight="1">
       <c r="A222" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>344</v>
+        <v>316</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="15" customHeight="1">
       <c r="A223" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="15" customHeight="1">
       <c r="A224" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>314</v>
@@ -6120,12 +6126,12 @@
         <v>343</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15" customHeight="1">
       <c r="A225" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>314</v>
@@ -6134,12 +6140,12 @@
         <v>343</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="15" customHeight="1">
       <c r="A226" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>314</v>
@@ -6148,12 +6154,12 @@
         <v>343</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15" customHeight="1">
       <c r="A227" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>314</v>
@@ -6162,12 +6168,12 @@
         <v>343</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15" customHeight="1">
       <c r="A228" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>314</v>
@@ -6176,12 +6182,12 @@
         <v>343</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="15" customHeight="1">
       <c r="A229" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>314</v>
@@ -6190,12 +6196,12 @@
         <v>343</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="15" customHeight="1">
       <c r="A230" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>314</v>
@@ -6204,12 +6210,12 @@
         <v>343</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="15" customHeight="1">
       <c r="A231" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>314</v>
@@ -6218,12 +6224,12 @@
         <v>343</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="15" customHeight="1">
       <c r="A232" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>314</v>
@@ -6232,12 +6238,12 @@
         <v>343</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15" customHeight="1">
       <c r="A233" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>314</v>
@@ -6246,12 +6252,12 @@
         <v>343</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="234" spans="1:4" ht="15" customHeight="1">
       <c r="A234" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>314</v>
@@ -6260,12 +6266,12 @@
         <v>343</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="15" customHeight="1">
       <c r="A235" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>314</v>
@@ -6274,12 +6280,12 @@
         <v>343</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15" customHeight="1">
       <c r="A236" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>314</v>
@@ -6288,12 +6294,12 @@
         <v>343</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15" customHeight="1">
       <c r="A237" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>314</v>
@@ -6302,12 +6308,12 @@
         <v>343</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15" customHeight="1">
       <c r="A238" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>314</v>
@@ -6316,12 +6322,12 @@
         <v>343</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15" customHeight="1">
       <c r="A239" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>314</v>
@@ -6330,12 +6336,12 @@
         <v>343</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="15" customHeight="1">
       <c r="A240" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>314</v>
@@ -6344,54 +6350,54 @@
         <v>343</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="15" customHeight="1">
       <c r="A241" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>316</v>
+        <v>343</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="15" customHeight="1">
       <c r="A242" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="243" spans="1:4" ht="15" customHeight="1">
       <c r="A243" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B243" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15" customHeight="1">
       <c r="A244" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>314</v>
@@ -6400,12 +6406,12 @@
         <v>343</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="15" customHeight="1">
       <c r="A245" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B245" s="2" t="s">
         <v>314</v>
@@ -6414,12 +6420,12 @@
         <v>343</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="15" customHeight="1">
       <c r="A246" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B246" s="2" t="s">
         <v>314</v>
@@ -6428,12 +6434,12 @@
         <v>343</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="15" customHeight="1">
       <c r="A247" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>314</v>
@@ -6442,12 +6448,12 @@
         <v>343</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="15" customHeight="1">
       <c r="A248" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>314</v>
@@ -6456,12 +6462,12 @@
         <v>343</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="15" customHeight="1">
       <c r="A249" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B249" s="2" t="s">
         <v>314</v>
@@ -6470,12 +6476,12 @@
         <v>343</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="15" customHeight="1">
       <c r="A250" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>314</v>
@@ -6484,12 +6490,12 @@
         <v>343</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="15" customHeight="1">
       <c r="A251" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>314</v>
@@ -6498,12 +6504,12 @@
         <v>343</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15" customHeight="1">
       <c r="A252" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>314</v>
@@ -6512,12 +6518,12 @@
         <v>343</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15" customHeight="1">
       <c r="A253" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>314</v>
@@ -6526,12 +6532,12 @@
         <v>343</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15" customHeight="1">
       <c r="A254" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>314</v>
@@ -6540,12 +6546,12 @@
         <v>343</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15" customHeight="1">
       <c r="A255" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>314</v>
@@ -6554,12 +6560,12 @@
         <v>343</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="15" customHeight="1">
       <c r="A256" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>314</v>
@@ -6568,12 +6574,12 @@
         <v>343</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="15" customHeight="1">
       <c r="A257" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>314</v>
@@ -6582,12 +6588,12 @@
         <v>343</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="15" customHeight="1">
       <c r="A258" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>314</v>
@@ -6596,12 +6602,12 @@
         <v>343</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="15" customHeight="1">
       <c r="A259" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>314</v>
@@ -6610,12 +6616,12 @@
         <v>343</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="15" customHeight="1">
       <c r="A260" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>314</v>
@@ -6624,96 +6630,96 @@
         <v>343</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="15" customHeight="1">
       <c r="A261" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>316</v>
+        <v>343</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="15" customHeight="1">
       <c r="A262" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="15" customHeight="1">
       <c r="A263" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>345</v>
+        <v>317</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="15" customHeight="1">
       <c r="A264" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="15" customHeight="1">
       <c r="A265" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15" customHeight="1">
       <c r="A266" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15" customHeight="1">
       <c r="A267" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>314</v>
@@ -6722,12 +6728,12 @@
         <v>348</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15" customHeight="1">
       <c r="A268" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>314</v>
@@ -6736,116 +6742,116 @@
         <v>348</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="15" customHeight="1">
       <c r="A269" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="15" customHeight="1">
       <c r="A270" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15" customHeight="1">
       <c r="A271" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="15" customHeight="1">
       <c r="A272" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="15" customHeight="1">
       <c r="A273" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="15" customHeight="1">
       <c r="A274" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="15" customHeight="1">
       <c r="A275" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="15" customHeight="1">
       <c r="A276" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D276" s="2" t="s">
         <v>626</v>
@@ -6853,21 +6859,21 @@
     </row>
     <row r="277" spans="1:4" ht="15" customHeight="1">
       <c r="A277" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="15" customHeight="1">
       <c r="A278" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B278" s="2" t="s">
         <v>314</v>
@@ -6876,12 +6882,12 @@
         <v>348</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="15" customHeight="1">
       <c r="A279" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B279" s="2" t="s">
         <v>314</v>
@@ -6890,32 +6896,32 @@
         <v>348</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="15" customHeight="1">
       <c r="A280" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B280" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="15" customHeight="1">
       <c r="A281" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>630</v>
@@ -6923,27 +6929,27 @@
     </row>
     <row r="282" spans="1:4" ht="15" customHeight="1">
       <c r="A282" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="15" customHeight="1">
       <c r="A283" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D283" s="2" t="s">
         <v>631</v>
@@ -6951,55 +6957,55 @@
     </row>
     <row r="284" spans="1:4" ht="15" customHeight="1">
       <c r="A284" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="15" customHeight="1">
       <c r="A285" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B285" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="286" spans="1:4" ht="15" customHeight="1">
       <c r="A286" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15" customHeight="1">
       <c r="A287" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>634</v>
@@ -7007,21 +7013,21 @@
     </row>
     <row r="288" spans="1:4" ht="15" customHeight="1">
       <c r="A288" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>617</v>
+        <v>634</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="15" customHeight="1">
       <c r="A289" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B289" s="2" t="s">
         <v>314</v>
@@ -7030,12 +7036,12 @@
         <v>348</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>635</v>
+        <v>617</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="15" customHeight="1">
       <c r="A290" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>314</v>
@@ -7044,32 +7050,32 @@
         <v>348</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="15" customHeight="1">
       <c r="A291" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="15" customHeight="1">
       <c r="A292" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>637</v>
@@ -7077,27 +7083,27 @@
     </row>
     <row r="293" spans="1:4" ht="15" customHeight="1">
       <c r="A293" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="15" customHeight="1">
       <c r="A294" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>638</v>
@@ -7105,35 +7111,35 @@
     </row>
     <row r="295" spans="1:4" ht="15" customHeight="1">
       <c r="A295" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="15" customHeight="1">
       <c r="A296" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>316</v>
+        <v>349</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15" customHeight="1">
       <c r="A297" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>313</v>
@@ -7142,26 +7148,26 @@
         <v>316</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="15" customHeight="1">
       <c r="A298" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>350</v>
+        <v>316</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15" customHeight="1">
       <c r="A299" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>314</v>
@@ -7170,12 +7176,12 @@
         <v>350</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="15" customHeight="1">
       <c r="A300" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>314</v>
@@ -7184,26 +7190,26 @@
         <v>350</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15" customHeight="1">
       <c r="A301" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15" customHeight="1">
       <c r="A302" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>314</v>
@@ -7212,26 +7218,26 @@
         <v>351</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15" customHeight="1">
       <c r="A303" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="15" customHeight="1">
       <c r="A304" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>314</v>
@@ -7240,12 +7246,12 @@
         <v>350</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15" customHeight="1">
       <c r="A305" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>314</v>
@@ -7254,12 +7260,12 @@
         <v>350</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="15" customHeight="1">
       <c r="A306" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B306" s="2" t="s">
         <v>314</v>
@@ -7268,26 +7274,26 @@
         <v>350</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="15" customHeight="1">
       <c r="A307" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B307" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="15" customHeight="1">
       <c r="A308" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>314</v>
@@ -7296,40 +7302,40 @@
         <v>351</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="15" customHeight="1">
       <c r="A309" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B309" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="15" customHeight="1">
       <c r="A310" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>316</v>
+        <v>350</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="15" customHeight="1">
       <c r="A311" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>313</v>
@@ -7338,12 +7344,12 @@
         <v>316</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="15" customHeight="1">
       <c r="A312" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>313</v>
@@ -7352,96 +7358,96 @@
         <v>316</v>
       </c>
       <c r="D312" s="2" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" ht="15" customHeight="1">
+      <c r="A313" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D313" s="2" t="s">
         <v>650</v>
-      </c>
-    </row>
-    <row r="313" spans="1:4" ht="15" customHeight="1">
-      <c r="A313" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B313" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C313" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="D313" s="3" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="15" customHeight="1">
       <c r="A314" s="4" t="s">
-        <v>824</v>
+        <v>104</v>
       </c>
       <c r="B314" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="C314" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="D314" s="5" t="s">
-        <v>818</v>
+      <c r="C314" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D314" s="3" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="15" customHeight="1">
       <c r="A315" s="4" t="s">
-        <v>823</v>
-      </c>
-      <c r="B315" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="B315" s="3" t="s">
         <v>313</v>
       </c>
       <c r="C315" s="5" t="s">
-        <v>822</v>
-      </c>
-      <c r="D315" s="3" t="s">
-        <v>817</v>
+        <v>316</v>
+      </c>
+      <c r="D315" s="5" t="s">
+        <v>818</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="15" customHeight="1">
       <c r="A316" s="4" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B316" s="4" t="s">
         <v>313</v>
       </c>
       <c r="C316" s="5" t="s">
-        <v>316</v>
+        <v>822</v>
       </c>
       <c r="D316" s="3" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="15" customHeight="1">
       <c r="A317" s="4" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B317" s="4" t="s">
         <v>313</v>
       </c>
       <c r="C317" s="5" t="s">
-        <v>821</v>
+        <v>316</v>
       </c>
       <c r="D317" s="3" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="318" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A318" s="6" t="s">
-        <v>827</v>
+        <v>819</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" ht="15" customHeight="1">
+      <c r="A318" s="4" t="s">
+        <v>826</v>
       </c>
       <c r="B318" s="4" t="s">
         <v>313</v>
       </c>
       <c r="C318" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="D318" s="8" t="s">
-        <v>835</v>
+        <v>821</v>
+      </c>
+      <c r="D318" s="3" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="319" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A319" s="6" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B319" s="4" t="s">
         <v>313</v>
@@ -7450,12 +7456,12 @@
         <v>316</v>
       </c>
       <c r="D319" s="8" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="320" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A320" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B320" s="4" t="s">
         <v>313</v>
@@ -7463,13 +7469,13 @@
       <c r="C320" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="D320" s="7" t="s">
-        <v>837</v>
+      <c r="D320" s="8" t="s">
+        <v>836</v>
       </c>
     </row>
     <row r="321" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A321" s="6" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B321" s="4" t="s">
         <v>313</v>
@@ -7478,12 +7484,12 @@
         <v>316</v>
       </c>
       <c r="D321" s="7" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="322" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A322" s="7" t="s">
-        <v>831</v>
+      <c r="A322" s="6" t="s">
+        <v>830</v>
       </c>
       <c r="B322" s="4" t="s">
         <v>313</v>
@@ -7492,12 +7498,12 @@
         <v>316</v>
       </c>
       <c r="D322" s="7" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="323" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A323" s="7" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B323" s="4" t="s">
         <v>313</v>
@@ -7506,12 +7512,12 @@
         <v>316</v>
       </c>
       <c r="D323" s="7" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="324" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A324" s="7" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B324" s="4" t="s">
         <v>313</v>
@@ -7520,12 +7526,12 @@
         <v>316</v>
       </c>
       <c r="D324" s="7" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="325" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A325" s="7" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B325" s="4" t="s">
         <v>313</v>
@@ -7534,26 +7540,26 @@
         <v>316</v>
       </c>
       <c r="D325" s="7" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A326" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="B326" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C326" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D326" s="7" t="s">
         <v>842</v>
-      </c>
-    </row>
-    <row r="326" spans="1:4" ht="15" customHeight="1">
-      <c r="A326" s="1" t="s">
-        <v>844</v>
-      </c>
-      <c r="B326" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C326" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D326" s="1" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="327" spans="1:4" ht="15" customHeight="1">
       <c r="A327" s="1" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>313</v>
@@ -7562,12 +7568,12 @@
         <v>316</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="15" customHeight="1">
       <c r="A328" s="1" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>313</v>
@@ -7576,6 +7582,20 @@
         <v>316</v>
       </c>
       <c r="D328" s="1" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" ht="15" customHeight="1">
+      <c r="A329" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D329" s="1" t="s">
         <v>849</v>
       </c>
     </row>
@@ -7591,9 +7611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D327"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D316" sqref="D316"/>
+      <selection pane="bottomLeft" activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="15" customHeight="1"/>

</xml_diff>